<commit_message>
Concentrado de metricas Julio
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150730.xlsx
+++ b/qualtcom/Organizacional/Medicion y Monitoreo/Concentrado_Métricas-150730.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="1470" yWindow="0" windowWidth="16605" windowHeight="9435" tabRatio="835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Funcional" sheetId="11" r:id="rId6"/>
     <sheet name="Indice de Satisfacción" sheetId="13" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -530,9 +530,6 @@
     <xf numFmtId="9" fontId="8" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="5" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,6 +594,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="8" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -700,42 +700,7 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
     <cellStyle name="Porcentaje 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="109">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="104">
     <dxf>
       <fill>
         <patternFill>
@@ -1712,11 +1677,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="4198240"/>
-        <c:axId val="4198800"/>
+        <c:axId val="205401024"/>
+        <c:axId val="205401584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4198240"/>
+        <c:axId val="205401024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1726,7 +1691,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4198800"/>
+        <c:crossAx val="205401584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1734,7 +1699,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4198800"/>
+        <c:axId val="205401584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1710,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4198240"/>
+        <c:crossAx val="205401024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1797,7 +1762,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1861,11 +1825,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168747760"/>
-        <c:axId val="168748320"/>
+        <c:axId val="217996272"/>
+        <c:axId val="217996832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168747760"/>
+        <c:axId val="217996272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1875,7 +1839,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168748320"/>
+        <c:crossAx val="217996832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1883,7 +1847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168748320"/>
+        <c:axId val="217996832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1895,7 +1859,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168747760"/>
+        <c:crossAx val="217996272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1953,7 +1917,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2306,11 +2269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="193783920"/>
-        <c:axId val="193784480"/>
+        <c:axId val="268114448"/>
+        <c:axId val="268115008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="193783920"/>
+        <c:axId val="268114448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2320,7 +2283,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193784480"/>
+        <c:crossAx val="268115008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2328,7 +2291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193784480"/>
+        <c:axId val="268115008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2340,7 +2303,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193783920"/>
+        <c:crossAx val="268114448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2512,11 +2475,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144137008"/>
-        <c:axId val="144137568"/>
+        <c:axId val="205404384"/>
+        <c:axId val="205404944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144137008"/>
+        <c:axId val="205404384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2526,7 +2489,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144137568"/>
+        <c:crossAx val="205404944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2534,7 +2497,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144137568"/>
+        <c:axId val="205404944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2547,7 +2510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144137008"/>
+        <c:crossAx val="205404384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2713,11 +2676,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144140368"/>
-        <c:axId val="144140928"/>
+        <c:axId val="205407744"/>
+        <c:axId val="205408304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144140368"/>
+        <c:axId val="205407744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2727,7 +2690,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144140928"/>
+        <c:crossAx val="205408304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2735,7 +2698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144140928"/>
+        <c:axId val="205408304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2746,7 +2709,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144140368"/>
+        <c:crossAx val="205407744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2867,11 +2830,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144491696"/>
-        <c:axId val="144492256"/>
+        <c:axId val="205653872"/>
+        <c:axId val="205654432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144491696"/>
+        <c:axId val="205653872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2881,7 +2844,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144492256"/>
+        <c:crossAx val="205654432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2889,7 +2852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144492256"/>
+        <c:axId val="205654432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2902,7 +2865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144491696"/>
+        <c:crossAx val="205653872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3013,11 +2976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144494496"/>
-        <c:axId val="144495056"/>
+        <c:axId val="136418320"/>
+        <c:axId val="136418880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144494496"/>
+        <c:axId val="136418320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3027,7 +2990,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144495056"/>
+        <c:crossAx val="136418880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3035,7 +2998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144495056"/>
+        <c:axId val="136418880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3046,7 +3009,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144494496"/>
+        <c:crossAx val="136418320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3140,7 +3103,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -3163,11 +3126,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144497856"/>
-        <c:axId val="96038720"/>
+        <c:axId val="136421680"/>
+        <c:axId val="136422240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144497856"/>
+        <c:axId val="136421680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3177,7 +3140,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96038720"/>
+        <c:crossAx val="136422240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3185,7 +3148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96038720"/>
+        <c:axId val="136422240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3197,7 +3160,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144497856"/>
+        <c:crossAx val="136421680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3250,7 +3213,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3320,11 +3282,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="96041520"/>
-        <c:axId val="96042080"/>
+        <c:axId val="217949536"/>
+        <c:axId val="217950096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96041520"/>
+        <c:axId val="217949536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3334,7 +3296,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96042080"/>
+        <c:crossAx val="217950096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3342,7 +3304,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96042080"/>
+        <c:axId val="217950096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3354,7 +3316,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96041520"/>
+        <c:crossAx val="217949536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3407,7 +3369,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3471,11 +3432,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="96044880"/>
-        <c:axId val="96045440"/>
+        <c:axId val="217952896"/>
+        <c:axId val="217990112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96044880"/>
+        <c:axId val="217952896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3485,7 +3446,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96045440"/>
+        <c:crossAx val="217990112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3493,7 +3454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96045440"/>
+        <c:axId val="217990112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3505,7 +3466,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96044880"/>
+        <c:crossAx val="217952896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3622,11 +3583,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="168744400"/>
-        <c:axId val="168744960"/>
+        <c:axId val="217992912"/>
+        <c:axId val="217993472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="168744400"/>
+        <c:axId val="217992912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3636,7 +3597,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168744960"/>
+        <c:crossAx val="217993472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3644,7 +3605,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="168744960"/>
+        <c:axId val="217993472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3656,7 +3617,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168744400"/>
+        <c:crossAx val="217992912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4403,7 +4364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -4440,7 +4401,7 @@
     <row r="17" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:22" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:22" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="37" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="16" t="s">
@@ -4460,13 +4421,13 @@
       <c r="C20" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="36">
         <v>160</v>
       </c>
-      <c r="E20" s="37">
+      <c r="E20" s="36">
         <v>135</v>
       </c>
-      <c r="F20" s="48">
+      <c r="F20" s="47">
         <f>(D20-E20)/D20</f>
         <v>0.15625</v>
       </c>
@@ -4476,13 +4437,13 @@
       <c r="C21" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="36">
         <v>60</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="36">
         <v>17.899999999999999</v>
       </c>
-      <c r="F21" s="40">
+      <c r="F21" s="39">
         <f t="shared" ref="F21:F26" si="0">(D21-E21)/D21</f>
         <v>0.70166666666666666</v>
       </c>
@@ -4494,13 +4455,13 @@
       <c r="C22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="36">
         <v>91.2</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="36">
         <v>92.3</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="39">
         <f t="shared" si="0"/>
         <v>-1.2061403508771867E-2</v>
       </c>
@@ -4510,61 +4471,61 @@
       <c r="C23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="36">
         <v>45.2</v>
       </c>
-      <c r="E23" s="37">
+      <c r="E23" s="36">
         <v>9.69</v>
       </c>
-      <c r="F23" s="51">
+      <c r="F23" s="50">
         <f>(D23-E23)/D23</f>
         <v>0.78561946902654878</v>
       </c>
     </row>
     <row r="24" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="36">
-        <v>1</v>
-      </c>
-      <c r="E24" s="36">
-        <v>1</v>
-      </c>
-      <c r="F24" s="41">
+      <c r="C24" s="34"/>
+      <c r="D24" s="35">
+        <v>1</v>
+      </c>
+      <c r="E24" s="35">
+        <v>1</v>
+      </c>
+      <c r="F24" s="40">
         <f>(D24-E24)/D24</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36">
+      <c r="C25" s="34"/>
+      <c r="D25" s="35">
         <v>2</v>
       </c>
-      <c r="E25" s="36">
+      <c r="E25" s="35">
         <v>2</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F25" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:22" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36">
+      <c r="C26" s="34"/>
+      <c r="D26" s="35">
         <v>0.5</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="38">
         <v>0.5</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5053,21 +5014,21 @@
     <mergeCell ref="B20:B21"/>
   </mergeCells>
   <conditionalFormatting sqref="A29:XFD1048576">
-    <cfRule type="cellIs" dxfId="108" priority="66" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="103" priority="66" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="107" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="3" operator="lessThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="cellIs" dxfId="106" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="101" priority="1" operator="between">
       <formula>0.31</formula>
       <formula>0.6599</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="100" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
@@ -5147,7 +5108,7 @@
         <f>PRODUCT(('Desviacion de esfuerzo'!E20 + 'Desviacion de esfuerzo'!E21),41.62)</f>
         <v>6363.6979999999994</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="49">
         <f>(C20-D20)/C20</f>
         <v>0.36292942236460113</v>
       </c>
@@ -5163,7 +5124,7 @@
         <f>PRODUCT(('Desviacion de esfuerzo'!E22 + 'Desviacion de esfuerzo'!E23),41.62)</f>
         <v>4244.8237999999992</v>
       </c>
-      <c r="E21" s="49">
+      <c r="E21" s="48">
         <f>(C21-D21)/C21</f>
         <v>0.25447399156616157</v>
       </c>
@@ -5180,34 +5141,34 @@
     <row r="31" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A27:XFD1048576">
-    <cfRule type="cellIs" dxfId="104" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="99" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison5!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="103" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="98" priority="4" operator="between">
       <formula>0.66</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="97" priority="5" stopIfTrue="1" operator="between">
       <formula>0.31</formula>
       <formula>0.65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="6" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="96" priority="6" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="100" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="95" priority="1" operator="between">
       <formula>0.66</formula>
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="94" priority="2" operator="between">
       <formula>0.31</formula>
       <formula>0.65</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="93" priority="3" operator="between">
       <formula>0</formula>
       <formula>0.3</formula>
     </cfRule>
@@ -5224,7 +5185,7 @@
   <dimension ref="B2:R25"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5271,7 +5232,7 @@
       <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>150228</v>
       </c>
       <c r="E3" s="17">
@@ -5316,7 +5277,7 @@
       <c r="I4" s="22">
         <v>1</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="41">
         <f>AVERAGE(D4:I4)</f>
         <v>1</v>
       </c>
@@ -5346,7 +5307,7 @@
       <c r="I5" s="22">
         <v>1</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="41">
         <f>AVERAGE(D5:I5)</f>
         <v>0.96</v>
       </c>
@@ -5409,7 +5370,7 @@
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>150227</v>
       </c>
       <c r="E9" s="17">
@@ -5449,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="23"/>
-      <c r="J10" s="27">
+      <c r="J10" s="42">
         <f>AVERAGE(D10:H10)</f>
         <v>1</v>
       </c>
@@ -5470,10 +5431,12 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="27" t="e">
-        <f t="shared" ref="J11" si="0">AVERAGE(D11:F11)</f>
-        <v>#DIV/0!</v>
+      <c r="I11" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="J11" s="51">
+        <f>AVERAGE(D11:I11)</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
@@ -5495,7 +5458,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="23"/>
-      <c r="J12" s="27">
+      <c r="J12" s="42">
         <f>AVERAGE(D12:H12)</f>
         <v>1</v>
       </c>
@@ -5503,87 +5466,87 @@
     <row r="25" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A3:C3 P2:XFD6 A9:A12 A15:XFD1048576 A8:B8 A4:J6 A2:E2 A7:K7 K8 A13:K14 M7:XFD14 J9:K12 J2">
-    <cfRule type="cellIs" dxfId="97" priority="24" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="92" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="96" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="91" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="95" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="90" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="94" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="89" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="93" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="88" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:I12">
-    <cfRule type="cellIs" dxfId="92" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="87" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:C12">
-    <cfRule type="cellIs" dxfId="91" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="86" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="90" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="85" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="89" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="84" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="88" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="83" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="87" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="82" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="86" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="81" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="85" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="80" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:I2">
-    <cfRule type="cellIs" dxfId="84" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="79" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:I3">
-    <cfRule type="cellIs" dxfId="83" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="78" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:I8">
-    <cfRule type="cellIs" dxfId="82" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="77" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9:I9">
-    <cfRule type="cellIs" dxfId="81" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="76" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5650,7 +5613,7 @@
       <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>150228</v>
       </c>
       <c r="E3" s="17">
@@ -5697,7 +5660,7 @@
       <c r="I4" s="23">
         <v>1</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f>AVERAGE(D4:I4)</f>
         <v>1</v>
       </c>
@@ -5729,7 +5692,7 @@
       <c r="I5" s="23">
         <v>1</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="42">
         <f>AVERAGE(D5:I5)</f>
         <v>1</v>
       </c>
@@ -5761,7 +5724,7 @@
       <c r="I6" s="23">
         <v>1</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="42">
         <f>AVERAGE(D6:I6)</f>
         <v>1</v>
       </c>
@@ -5793,7 +5756,7 @@
       <c r="I7" s="23">
         <v>1</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="42">
         <f>AVERAGE(D7:I7)</f>
         <v>1</v>
       </c>
@@ -5801,25 +5764,25 @@
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="J8" s="34"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="J8" s="33"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -5834,7 +5797,7 @@
       <c r="I9" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="27" t="s">
         <v>7</v>
       </c>
       <c r="K9" s="7"/>
@@ -5843,7 +5806,7 @@
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>150227</v>
       </c>
       <c r="E10" s="17">
@@ -5886,7 +5849,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="22"/>
-      <c r="J11" s="42">
+      <c r="J11" s="41">
         <f>AVERAGE(D11:H11)</f>
         <v>1</v>
       </c>
@@ -5914,7 +5877,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="22"/>
-      <c r="J12" s="42">
+      <c r="J12" s="41">
         <f>AVERAGE(D12:H12)</f>
         <v>1</v>
       </c>
@@ -5982,182 +5945,182 @@
     <sortCondition descending="1" ref="C29"/>
   </sortState>
   <conditionalFormatting sqref="M2:XFD11 A2:A12 K2:L3 K12:XFD12 A14:H15 A19:H1048576 A16:B18 D16:H18 J14:XFD1048576">
-    <cfRule type="cellIs" dxfId="80" priority="46" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="75" priority="46" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B9 B2:D2 J10:J13 C4:H6 J2 J4:J6">
-    <cfRule type="cellIs" dxfId="79" priority="45" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="74" priority="45" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="78" priority="42" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="73" priority="42" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="77" priority="43" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="72" priority="43" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="76" priority="36" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="71" priority="36" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11:D13">
-    <cfRule type="cellIs" dxfId="75" priority="40" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="70" priority="40" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="74" priority="39" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="69" priority="39" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C13">
-    <cfRule type="cellIs" dxfId="73" priority="35" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="68" priority="35" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="72" priority="34" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="67" priority="34" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B13">
-    <cfRule type="cellIs" dxfId="71" priority="33" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="66" priority="33" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:H13">
-    <cfRule type="cellIs" dxfId="70" priority="30" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="65" priority="30" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="69" priority="29" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="64" priority="29" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="68" priority="27" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="63" priority="27" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="67" priority="26" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="62" priority="26" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="66" priority="24" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="61" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="65" priority="22" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="60" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="64" priority="21" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="59" priority="21" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:H8 J7:J8">
-    <cfRule type="cellIs" dxfId="63" priority="20" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="58" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B8">
-    <cfRule type="cellIs" dxfId="62" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="57" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="61" priority="18" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="56" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="60" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="55" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="cellIs" dxfId="59" priority="16" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="54" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G3">
-    <cfRule type="cellIs" dxfId="58" priority="15" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="53" priority="15" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="57" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="52" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="cellIs" dxfId="56" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="51" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="cellIs" dxfId="55" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="50" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="54" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="49" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="53" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="48" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="52" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="47" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I6">
-    <cfRule type="cellIs" dxfId="51" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="46" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="50" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="45" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="49" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="44" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I13">
-    <cfRule type="cellIs" dxfId="48" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="43" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="47" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="42" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="46" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="41" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="45" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="40" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6175,7 +6138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -6194,7 +6157,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -6212,7 +6175,7 @@
       <c r="I2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="7"/>
@@ -6223,7 +6186,7 @@
       <c r="C3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>150227</v>
       </c>
       <c r="E3" s="17">
@@ -6270,7 +6233,7 @@
       <c r="I4" s="23">
         <v>1</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f>AVERAGE(D4:I4)</f>
         <v>1</v>
       </c>
@@ -6302,7 +6265,7 @@
       <c r="I5" s="23">
         <v>1</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="42">
         <f>AVERAGE(D5:H5)</f>
         <v>1</v>
       </c>
@@ -6332,7 +6295,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="23"/>
-      <c r="J6" s="43">
+      <c r="J6" s="42">
         <f>AVERAGE(D6:H6)</f>
         <v>1</v>
       </c>
@@ -6378,67 +6341,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7 K2:L3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12 L7:XFD7 M2:XFD6">
-    <cfRule type="cellIs" dxfId="44" priority="26" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="39" priority="26" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:I7 J2 C4:E6 G4:J6">
-    <cfRule type="cellIs" dxfId="43" priority="25" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="25" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="42" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="37" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="41" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="40" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="35" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="39" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="34" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="33" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="37" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="32" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="cellIs" dxfId="36" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="30" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="34" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I2">
-    <cfRule type="cellIs" dxfId="33" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I3">
-    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6470,7 +6433,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>32</v>
       </c>
       <c r="E2" s="21" t="s">
@@ -6488,7 +6451,7 @@
       <c r="I2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="7"/>
@@ -6499,7 +6462,7 @@
       <c r="C3" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="28">
         <v>150227</v>
       </c>
       <c r="E3" s="17">
@@ -6546,7 +6509,7 @@
       <c r="I4" s="23">
         <v>1</v>
       </c>
-      <c r="J4" s="43">
+      <c r="J4" s="42">
         <f>AVERAGE(D4:I4)</f>
         <v>0.95833333333333337</v>
       </c>
@@ -6578,7 +6541,7 @@
       <c r="I5" s="23">
         <v>1</v>
       </c>
-      <c r="J5" s="43">
+      <c r="J5" s="42">
         <f>AVERAGE(D5:I5)</f>
         <v>1</v>
       </c>
@@ -6610,7 +6573,7 @@
       <c r="I6" s="23">
         <v>1</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="42">
         <f>AVERAGE(D6:I6)</f>
         <v>1</v>
       </c>
@@ -6656,82 +6619,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7 K2:L3 A8:XFD9 A13:XFD1048576 A10:B12 D10:XFD12 L7:XFD7 M2:XFD6">
-    <cfRule type="cellIs" dxfId="31" priority="19" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="26" priority="19" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison2!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3 B2:D2 B7:I7 J2 C4:E6 G4:H6 J4:J6">
-    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="25" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B6">
-    <cfRule type="cellIs" dxfId="29" priority="17" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="24" priority="17" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="23" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="27" priority="13" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="22" priority="13" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="26" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="21" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="25" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="24" priority="9" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="19" priority="9" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F6">
-    <cfRule type="cellIs" dxfId="23" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="18" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="22" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="21" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="16" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:I2">
-    <cfRule type="cellIs" dxfId="20" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:I3">
-    <cfRule type="cellIs" dxfId="19" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6744,7 +6707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -6756,44 +6719,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="45" t="s">
+      <c r="I2" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="44" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="29">
+      <c r="E3" s="28">
         <v>150227</v>
       </c>
       <c r="F3" s="17">
         <v>150331</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="28">
         <v>150430</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>150529</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="46">
         <v>150626</v>
       </c>
-      <c r="J3" s="47">
+      <c r="J3" s="46">
         <v>150730</v>
       </c>
     </row>
@@ -6810,16 +6773,16 @@
       <c r="F4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="43">
         <v>0.88</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="43">
         <v>0.94</v>
       </c>
-      <c r="I4" s="46">
+      <c r="I4" s="45">
         <v>0.94</v>
       </c>
-      <c r="J4" s="46">
+      <c r="J4" s="45">
         <v>0.97</v>
       </c>
     </row>
@@ -6836,16 +6799,16 @@
       <c r="F5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="43">
         <v>0.91</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="43">
         <v>0.97</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="45">
         <v>0.97</v>
       </c>
-      <c r="J5" s="46">
+      <c r="J5" s="45">
         <v>1</v>
       </c>
     </row>
@@ -6862,16 +6825,16 @@
       <c r="F6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="44">
-        <v>1</v>
-      </c>
-      <c r="H6" s="44">
-        <v>1</v>
-      </c>
-      <c r="I6" s="46">
-        <v>1</v>
-      </c>
-      <c r="J6" s="46">
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+      <c r="H6" s="43">
+        <v>1</v>
+      </c>
+      <c r="I6" s="45">
+        <v>1</v>
+      </c>
+      <c r="J6" s="45">
         <v>1</v>
       </c>
     </row>
@@ -6888,72 +6851,72 @@
       <c r="F7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="43">
         <v>0.88</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="43">
         <v>0.94</v>
       </c>
-      <c r="I7" s="46">
-        <v>1</v>
-      </c>
-      <c r="J7" s="46">
+      <c r="I7" s="45">
+        <v>1</v>
+      </c>
+      <c r="J7" s="45">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3 C2:E2 D4:G6 G2">
-    <cfRule type="cellIs" dxfId="18" priority="12" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="10" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="17" priority="11" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="11" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="16" priority="10" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="14" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="13" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7">
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H6 H2">
-    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="notEqual">
       <formula>INDIRECT("Dummy_for_Comparison1!"&amp;ADDRESS(ROW(),COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>